<commit_message>
Saved PITcleanr Excel file that I received back from Yakima Nation. Re-saved some output within process_detections script, so it's ready for DABOM. Included a tag summary file now that the detections have been finalized.
</commit_message>
<xml_diff>
--- a/outgoing/PITcleanr/PRO_Steelhead_2019.xlsx
+++ b/outgoing/PITcleanr/PRO_Steelhead_2019.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seek/Documents/GitProjects/MyProjects/DabomYakimaSthd/outgoing/PITcleanr/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE110E2-6FE2-6241-88F3-089250D6A9BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25180" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProcCapHist" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ProcCapHist!$A$1:$P$362</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -2059,8 +2065,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2106,6 +2112,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2152,7 +2166,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2184,9 +2198,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2218,6 +2250,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2393,37 +2443,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P362"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="N1" sqref="N1:O1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="10.5" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="9" max="10" width="10.5" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="12" max="13" width="16.1640625" customWidth="1"/>
+    <col min="14" max="14" width="9.5" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2473,7 +2520,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -2514,7 +2561,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2561,7 +2608,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2608,7 +2655,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2655,7 +2702,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2702,7 +2749,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2749,7 +2796,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -2796,7 +2843,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -2837,7 +2884,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -2884,7 +2931,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -2931,7 +2978,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -2972,7 +3019,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -3019,7 +3066,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -3066,7 +3113,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -3113,7 +3160,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -3160,7 +3207,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -3207,7 +3254,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -3248,7 +3295,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -3289,7 +3336,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -3336,7 +3383,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>70</v>
       </c>
@@ -3383,7 +3430,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -3424,7 +3471,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -3471,7 +3518,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>80</v>
       </c>
@@ -3518,7 +3565,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -3559,7 +3606,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -3600,7 +3647,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>88</v>
       </c>
@@ -3647,7 +3694,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -3688,7 +3735,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>93</v>
       </c>
@@ -3735,7 +3782,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>93</v>
       </c>
@@ -3782,7 +3829,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>93</v>
       </c>
@@ -3829,7 +3876,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>103</v>
       </c>
@@ -3870,7 +3917,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>103</v>
       </c>
@@ -3917,7 +3964,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>108</v>
       </c>
@@ -3958,7 +4005,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>108</v>
       </c>
@@ -4005,7 +4052,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>108</v>
       </c>
@@ -4052,7 +4099,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>108</v>
       </c>
@@ -4099,7 +4146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>108</v>
       </c>
@@ -4146,7 +4193,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>116</v>
       </c>
@@ -4187,7 +4234,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>116</v>
       </c>
@@ -4234,7 +4281,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>116</v>
       </c>
@@ -4281,7 +4328,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>122</v>
       </c>
@@ -4322,7 +4369,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>122</v>
       </c>
@@ -4369,7 +4416,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>122</v>
       </c>
@@ -4416,7 +4463,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>122</v>
       </c>
@@ -4463,7 +4510,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>122</v>
       </c>
@@ -4504,7 +4551,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>130</v>
       </c>
@@ -4545,7 +4592,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>133</v>
       </c>
@@ -4586,7 +4633,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>133</v>
       </c>
@@ -4633,7 +4680,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>137</v>
       </c>
@@ -4674,7 +4721,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>137</v>
       </c>
@@ -4721,7 +4768,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>137</v>
       </c>
@@ -4768,7 +4815,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>141</v>
       </c>
@@ -4809,7 +4856,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>141</v>
       </c>
@@ -4856,7 +4903,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>141</v>
       </c>
@@ -4903,7 +4950,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>147</v>
       </c>
@@ -4944,7 +4991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>147</v>
       </c>
@@ -4991,7 +5038,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>147</v>
       </c>
@@ -5038,7 +5085,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>147</v>
       </c>
@@ -5079,7 +5126,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>152</v>
       </c>
@@ -5120,7 +5167,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>152</v>
       </c>
@@ -5167,7 +5214,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>152</v>
       </c>
@@ -5214,7 +5261,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>160</v>
       </c>
@@ -5255,7 +5302,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>160</v>
       </c>
@@ -5302,7 +5349,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>160</v>
       </c>
@@ -5349,7 +5396,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>166</v>
       </c>
@@ -5390,7 +5437,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>166</v>
       </c>
@@ -5437,7 +5484,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>166</v>
       </c>
@@ -5484,7 +5531,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>166</v>
       </c>
@@ -5531,7 +5578,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>166</v>
       </c>
@@ -5578,7 +5625,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>174</v>
       </c>
@@ -5619,7 +5666,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>174</v>
       </c>
@@ -5666,7 +5713,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>179</v>
       </c>
@@ -5707,7 +5754,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:15">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>179</v>
       </c>
@@ -5754,7 +5801,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>185</v>
       </c>
@@ -5795,7 +5842,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:15">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>185</v>
       </c>
@@ -5842,7 +5889,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>185</v>
       </c>
@@ -5889,7 +5936,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:15">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>185</v>
       </c>
@@ -5936,7 +5983,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>185</v>
       </c>
@@ -5983,7 +6030,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:15">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>192</v>
       </c>
@@ -6024,7 +6071,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:15">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>192</v>
       </c>
@@ -6071,7 +6118,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:15">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>192</v>
       </c>
@@ -6112,7 +6159,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:15">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>197</v>
       </c>
@@ -6153,7 +6200,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:15">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>200</v>
       </c>
@@ -6194,7 +6241,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="1:15">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>200</v>
       </c>
@@ -6241,7 +6288,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:15">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>200</v>
       </c>
@@ -6288,7 +6335,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="1:15">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>200</v>
       </c>
@@ -6329,7 +6376,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="1:15">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>207</v>
       </c>
@@ -6370,7 +6417,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="89" spans="1:15">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>209</v>
       </c>
@@ -6411,7 +6458,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:15">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>209</v>
       </c>
@@ -6458,7 +6505,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:15">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>209</v>
       </c>
@@ -6505,7 +6552,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="92" spans="1:15">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>209</v>
       </c>
@@ -6546,7 +6593,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="93" spans="1:15">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>216</v>
       </c>
@@ -6587,7 +6634,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:15">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>216</v>
       </c>
@@ -6634,7 +6681,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:15">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>216</v>
       </c>
@@ -6681,7 +6728,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:15">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>216</v>
       </c>
@@ -6728,7 +6775,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:15">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>216</v>
       </c>
@@ -6769,7 +6816,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:15">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>224</v>
       </c>
@@ -6810,7 +6857,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:15">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>224</v>
       </c>
@@ -6857,7 +6904,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:15">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>224</v>
       </c>
@@ -6904,7 +6951,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="1:15">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>224</v>
       </c>
@@ -6951,7 +6998,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:15">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>224</v>
       </c>
@@ -6998,7 +7045,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:15">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>224</v>
       </c>
@@ -7045,7 +7092,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="104" spans="1:15">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>224</v>
       </c>
@@ -7092,7 +7139,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:15">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>233</v>
       </c>
@@ -7133,7 +7180,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="106" spans="1:15">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>237</v>
       </c>
@@ -7174,7 +7221,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="1:15">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>237</v>
       </c>
@@ -7221,7 +7268,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="1:15">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>237</v>
       </c>
@@ -7268,7 +7315,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" spans="1:15">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>237</v>
       </c>
@@ -7315,7 +7362,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:15">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>237</v>
       </c>
@@ -7362,7 +7409,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="1:15">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>237</v>
       </c>
@@ -7409,7 +7456,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="112" spans="1:15">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>237</v>
       </c>
@@ -7456,7 +7503,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="113" spans="1:15">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>237</v>
       </c>
@@ -7503,7 +7550,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="114" spans="1:15">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>237</v>
       </c>
@@ -7550,7 +7597,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="115" spans="1:15">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>237</v>
       </c>
@@ -7597,7 +7644,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="116" spans="1:15">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>237</v>
       </c>
@@ -7644,7 +7691,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="117" spans="1:15">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>237</v>
       </c>
@@ -7691,7 +7738,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="118" spans="1:15">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>237</v>
       </c>
@@ -7738,7 +7785,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="119" spans="1:15">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>237</v>
       </c>
@@ -7785,7 +7832,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="120" spans="1:15">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>259</v>
       </c>
@@ -7826,7 +7873,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="121" spans="1:15">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>259</v>
       </c>
@@ -7873,7 +7920,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="122" spans="1:15">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>259</v>
       </c>
@@ -7920,7 +7967,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="123" spans="1:15">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>259</v>
       </c>
@@ -7967,7 +8014,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="124" spans="1:15">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>265</v>
       </c>
@@ -8008,7 +8055,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="125" spans="1:15">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>265</v>
       </c>
@@ -8055,7 +8102,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="126" spans="1:15">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>265</v>
       </c>
@@ -8102,7 +8149,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="127" spans="1:15">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>265</v>
       </c>
@@ -8149,7 +8196,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="128" spans="1:15">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>265</v>
       </c>
@@ -8196,7 +8243,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="129" spans="1:15">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>271</v>
       </c>
@@ -8237,7 +8284,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="130" spans="1:15">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>271</v>
       </c>
@@ -8284,7 +8331,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="131" spans="1:15">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>271</v>
       </c>
@@ -8331,7 +8378,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="132" spans="1:15">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>276</v>
       </c>
@@ -8372,7 +8419,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="133" spans="1:15">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>276</v>
       </c>
@@ -8419,7 +8466,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="134" spans="1:15">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>276</v>
       </c>
@@ -8466,7 +8513,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="135" spans="1:15">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>276</v>
       </c>
@@ -8513,7 +8560,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="136" spans="1:15">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>281</v>
       </c>
@@ -8554,7 +8601,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="137" spans="1:15">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>281</v>
       </c>
@@ -8601,7 +8648,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="1:15">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>281</v>
       </c>
@@ -8648,7 +8695,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="1:15">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>286</v>
       </c>
@@ -8689,7 +8736,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="140" spans="1:15">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>286</v>
       </c>
@@ -8736,7 +8783,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="141" spans="1:15">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>286</v>
       </c>
@@ -8777,7 +8824,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="142" spans="1:15">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>291</v>
       </c>
@@ -8818,7 +8865,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="143" spans="1:15">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>291</v>
       </c>
@@ -8865,7 +8912,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="144" spans="1:15">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>291</v>
       </c>
@@ -8912,7 +8959,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="145" spans="1:15">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>291</v>
       </c>
@@ -8959,7 +9006,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="146" spans="1:15">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>291</v>
       </c>
@@ -9006,7 +9053,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="147" spans="1:15">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>298</v>
       </c>
@@ -9047,7 +9094,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="148" spans="1:15">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>298</v>
       </c>
@@ -9094,7 +9141,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="149" spans="1:15">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>298</v>
       </c>
@@ -9141,7 +9188,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="150" spans="1:15">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>298</v>
       </c>
@@ -9188,7 +9235,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="151" spans="1:15">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>298</v>
       </c>
@@ -9235,7 +9282,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="152" spans="1:15">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>309</v>
       </c>
@@ -9276,7 +9323,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="153" spans="1:15">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>309</v>
       </c>
@@ -9323,7 +9370,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="154" spans="1:15">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>312</v>
       </c>
@@ -9364,7 +9411,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="155" spans="1:15">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>312</v>
       </c>
@@ -9411,7 +9458,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="156" spans="1:15">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>312</v>
       </c>
@@ -9458,7 +9505,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="157" spans="1:15">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>312</v>
       </c>
@@ -9505,7 +9552,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="158" spans="1:15">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>318</v>
       </c>
@@ -9546,7 +9593,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="159" spans="1:15">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>322</v>
       </c>
@@ -9587,7 +9634,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="160" spans="1:15">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>322</v>
       </c>
@@ -9634,7 +9681,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="161" spans="1:15">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>322</v>
       </c>
@@ -9681,7 +9728,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="162" spans="1:15">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>322</v>
       </c>
@@ -9728,7 +9775,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="163" spans="1:15">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>322</v>
       </c>
@@ -9775,7 +9822,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="164" spans="1:15">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>331</v>
       </c>
@@ -9816,7 +9863,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="165" spans="1:15">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>334</v>
       </c>
@@ -9857,7 +9904,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="166" spans="1:15">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>334</v>
       </c>
@@ -9904,7 +9951,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="167" spans="1:15">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>338</v>
       </c>
@@ -9945,7 +9992,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="168" spans="1:15">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>338</v>
       </c>
@@ -9992,7 +10039,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="169" spans="1:15">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>338</v>
       </c>
@@ -10039,7 +10086,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="170" spans="1:15">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>343</v>
       </c>
@@ -10074,7 +10121,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="171" spans="1:15">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>343</v>
       </c>
@@ -10115,7 +10162,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="172" spans="1:15">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>343</v>
       </c>
@@ -10153,7 +10200,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="173" spans="1:15">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>343</v>
       </c>
@@ -10194,7 +10241,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="174" spans="1:15">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>343</v>
       </c>
@@ -10235,7 +10282,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="175" spans="1:15">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>350</v>
       </c>
@@ -10276,7 +10323,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="176" spans="1:15">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>350</v>
       </c>
@@ -10323,7 +10370,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="177" spans="1:15">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>350</v>
       </c>
@@ -10370,7 +10417,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="178" spans="1:15">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>350</v>
       </c>
@@ -10417,7 +10464,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="179" spans="1:15">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>350</v>
       </c>
@@ -10464,7 +10511,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="180" spans="1:15">
+    <row r="180" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>350</v>
       </c>
@@ -10511,7 +10558,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="181" spans="1:15">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>350</v>
       </c>
@@ -10558,7 +10605,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="182" spans="1:15">
+    <row r="182" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>350</v>
       </c>
@@ -10605,7 +10652,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="183" spans="1:15">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>350</v>
       </c>
@@ -10652,7 +10699,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="184" spans="1:15">
+    <row r="184" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>350</v>
       </c>
@@ -10699,7 +10746,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="185" spans="1:15">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>350</v>
       </c>
@@ -10746,7 +10793,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="186" spans="1:15">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>350</v>
       </c>
@@ -10793,7 +10840,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="187" spans="1:15">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>350</v>
       </c>
@@ -10840,7 +10887,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="188" spans="1:15">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>350</v>
       </c>
@@ -10887,7 +10934,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="189" spans="1:15">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>350</v>
       </c>
@@ -10934,7 +10981,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="190" spans="1:15">
+    <row r="190" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>350</v>
       </c>
@@ -10981,7 +11028,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="191" spans="1:15">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>350</v>
       </c>
@@ -11028,7 +11075,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="192" spans="1:15">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>350</v>
       </c>
@@ -11075,7 +11122,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="193" spans="1:15">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>388</v>
       </c>
@@ -11116,7 +11163,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="194" spans="1:15">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>392</v>
       </c>
@@ -11157,7 +11204,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="195" spans="1:15">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>392</v>
       </c>
@@ -11204,7 +11251,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="196" spans="1:15">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>392</v>
       </c>
@@ -11251,7 +11298,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="197" spans="1:15">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>392</v>
       </c>
@@ -11298,7 +11345,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="198" spans="1:15">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>392</v>
       </c>
@@ -11345,7 +11392,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:15">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>398</v>
       </c>
@@ -11386,7 +11433,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:15">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>398</v>
       </c>
@@ -11433,7 +11480,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:15">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>398</v>
       </c>
@@ -11480,7 +11527,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:15">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>398</v>
       </c>
@@ -11527,7 +11574,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:15">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>398</v>
       </c>
@@ -11574,7 +11621,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:15">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>398</v>
       </c>
@@ -11621,7 +11668,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:15">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>398</v>
       </c>
@@ -11668,7 +11715,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:15">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>407</v>
       </c>
@@ -11703,7 +11750,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="207" spans="1:15">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>407</v>
       </c>
@@ -11744,7 +11791,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="208" spans="1:15">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>407</v>
       </c>
@@ -11782,7 +11829,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="209" spans="1:15">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>407</v>
       </c>
@@ -11823,7 +11870,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="210" spans="1:15">
+    <row r="210" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>421</v>
       </c>
@@ -11864,7 +11911,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:15">
+    <row r="211" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>421</v>
       </c>
@@ -11911,7 +11958,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:15">
+    <row r="212" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>421</v>
       </c>
@@ -11958,7 +12005,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:15">
+    <row r="213" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>421</v>
       </c>
@@ -12005,7 +12052,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="214" spans="1:15">
+    <row r="214" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>421</v>
       </c>
@@ -12052,7 +12099,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="215" spans="1:15">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>421</v>
       </c>
@@ -12099,7 +12146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="216" spans="1:15">
+    <row r="216" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>429</v>
       </c>
@@ -12140,7 +12187,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="217" spans="1:15">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>429</v>
       </c>
@@ -12187,7 +12234,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="218" spans="1:15">
+    <row r="218" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>433</v>
       </c>
@@ -12228,7 +12275,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="219" spans="1:15">
+    <row r="219" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>433</v>
       </c>
@@ -12275,7 +12322,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="220" spans="1:15">
+    <row r="220" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>436</v>
       </c>
@@ -12316,7 +12363,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="221" spans="1:15">
+    <row r="221" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>436</v>
       </c>
@@ -12363,7 +12410,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="222" spans="1:15">
+    <row r="222" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>436</v>
       </c>
@@ -12410,7 +12457,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="223" spans="1:15">
+    <row r="223" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>436</v>
       </c>
@@ -12457,7 +12504,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="224" spans="1:15">
+    <row r="224" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>436</v>
       </c>
@@ -12504,7 +12551,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="225" spans="1:15">
+    <row r="225" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>436</v>
       </c>
@@ -12551,7 +12598,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="226" spans="1:15">
+    <row r="226" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>449</v>
       </c>
@@ -12592,7 +12639,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="227" spans="1:15">
+    <row r="227" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>449</v>
       </c>
@@ -12639,7 +12686,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="228" spans="1:15">
+    <row r="228" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>452</v>
       </c>
@@ -12680,7 +12727,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="229" spans="1:15">
+    <row r="229" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>452</v>
       </c>
@@ -12727,7 +12774,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="230" spans="1:15">
+    <row r="230" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>452</v>
       </c>
@@ -12768,7 +12815,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="231" spans="1:15">
+    <row r="231" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>456</v>
       </c>
@@ -12809,7 +12856,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="232" spans="1:15">
+    <row r="232" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>456</v>
       </c>
@@ -12856,7 +12903,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="233" spans="1:15">
+    <row r="233" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>456</v>
       </c>
@@ -12903,7 +12950,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="234" spans="1:15">
+    <row r="234" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>462</v>
       </c>
@@ -12944,7 +12991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="235" spans="1:15">
+    <row r="235" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>462</v>
       </c>
@@ -12991,7 +13038,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="236" spans="1:15">
+    <row r="236" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>465</v>
       </c>
@@ -13032,7 +13079,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="237" spans="1:15">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>465</v>
       </c>
@@ -13079,7 +13126,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="238" spans="1:15">
+    <row r="238" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>465</v>
       </c>
@@ -13126,7 +13173,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="239" spans="1:15">
+    <row r="239" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>465</v>
       </c>
@@ -13173,7 +13220,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="240" spans="1:15">
+    <row r="240" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>471</v>
       </c>
@@ -13214,7 +13261,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="241" spans="1:15">
+    <row r="241" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>471</v>
       </c>
@@ -13261,7 +13308,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="242" spans="1:15">
+    <row r="242" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>474</v>
       </c>
@@ -13302,7 +13349,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="243" spans="1:15">
+    <row r="243" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>474</v>
       </c>
@@ -13349,7 +13396,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="244" spans="1:15">
+    <row r="244" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>474</v>
       </c>
@@ -13396,7 +13443,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="245" spans="1:15">
+    <row r="245" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>474</v>
       </c>
@@ -13443,7 +13490,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="246" spans="1:15">
+    <row r="246" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>481</v>
       </c>
@@ -13484,7 +13531,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="247" spans="1:15">
+    <row r="247" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>481</v>
       </c>
@@ -13531,7 +13578,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="248" spans="1:15">
+    <row r="248" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>481</v>
       </c>
@@ -13572,7 +13619,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="249" spans="1:15">
+    <row r="249" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>485</v>
       </c>
@@ -13613,7 +13660,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="250" spans="1:15">
+    <row r="250" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>488</v>
       </c>
@@ -13654,7 +13701,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="251" spans="1:15">
+    <row r="251" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>488</v>
       </c>
@@ -13701,7 +13748,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="252" spans="1:15">
+    <row r="252" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>488</v>
       </c>
@@ -13748,7 +13795,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="253" spans="1:15">
+    <row r="253" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>492</v>
       </c>
@@ -13789,7 +13836,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="254" spans="1:15">
+    <row r="254" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>492</v>
       </c>
@@ -13836,7 +13883,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="255" spans="1:15">
+    <row r="255" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>495</v>
       </c>
@@ -13877,7 +13924,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="256" spans="1:15">
+    <row r="256" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>495</v>
       </c>
@@ -13924,7 +13971,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="257" spans="1:15">
+    <row r="257" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>495</v>
       </c>
@@ -13965,7 +14012,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="258" spans="1:15">
+    <row r="258" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>499</v>
       </c>
@@ -14006,7 +14053,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="259" spans="1:15">
+    <row r="259" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>499</v>
       </c>
@@ -14053,7 +14100,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="260" spans="1:15">
+    <row r="260" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>499</v>
       </c>
@@ -14094,7 +14141,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="261" spans="1:15">
+    <row r="261" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>504</v>
       </c>
@@ -14135,7 +14182,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="262" spans="1:15">
+    <row r="262" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>506</v>
       </c>
@@ -14176,7 +14223,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="263" spans="1:15">
+    <row r="263" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>506</v>
       </c>
@@ -14223,7 +14270,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="264" spans="1:15">
+    <row r="264" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>506</v>
       </c>
@@ -14270,7 +14317,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="265" spans="1:15">
+    <row r="265" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>510</v>
       </c>
@@ -14311,7 +14358,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="266" spans="1:15">
+    <row r="266" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>510</v>
       </c>
@@ -14358,7 +14405,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="267" spans="1:15">
+    <row r="267" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>510</v>
       </c>
@@ -14405,7 +14452,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="268" spans="1:15">
+    <row r="268" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>515</v>
       </c>
@@ -14446,7 +14493,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="269" spans="1:15">
+    <row r="269" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>515</v>
       </c>
@@ -14493,7 +14540,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="270" spans="1:15">
+    <row r="270" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>518</v>
       </c>
@@ -14534,7 +14581,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="271" spans="1:15">
+    <row r="271" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>520</v>
       </c>
@@ -14575,7 +14622,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="272" spans="1:15">
+    <row r="272" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>520</v>
       </c>
@@ -14622,7 +14669,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="273" spans="1:15">
+    <row r="273" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>524</v>
       </c>
@@ -14663,7 +14710,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="274" spans="1:15">
+    <row r="274" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>527</v>
       </c>
@@ -14704,7 +14751,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="275" spans="1:15">
+    <row r="275" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>527</v>
       </c>
@@ -14751,7 +14798,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="276" spans="1:15">
+    <row r="276" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>527</v>
       </c>
@@ -14798,7 +14845,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="277" spans="1:15">
+    <row r="277" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>531</v>
       </c>
@@ -14839,7 +14886,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="278" spans="1:15">
+    <row r="278" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>534</v>
       </c>
@@ -14880,7 +14927,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="279" spans="1:15">
+    <row r="279" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>534</v>
       </c>
@@ -14927,7 +14974,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="280" spans="1:15">
+    <row r="280" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>538</v>
       </c>
@@ -14968,7 +15015,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="281" spans="1:15">
+    <row r="281" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>538</v>
       </c>
@@ -15015,7 +15062,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="282" spans="1:15">
+    <row r="282" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>538</v>
       </c>
@@ -15056,7 +15103,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="283" spans="1:15">
+    <row r="283" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>543</v>
       </c>
@@ -15097,7 +15144,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="284" spans="1:15">
+    <row r="284" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>543</v>
       </c>
@@ -15144,7 +15191,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="285" spans="1:15">
+    <row r="285" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>543</v>
       </c>
@@ -15191,7 +15238,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="286" spans="1:15">
+    <row r="286" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>543</v>
       </c>
@@ -15238,7 +15285,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="287" spans="1:15">
+    <row r="287" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>549</v>
       </c>
@@ -15279,7 +15326,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="288" spans="1:15">
+    <row r="288" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>549</v>
       </c>
@@ -15326,7 +15373,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="289" spans="1:15">
+    <row r="289" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>549</v>
       </c>
@@ -15373,7 +15420,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="290" spans="1:15">
+    <row r="290" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>549</v>
       </c>
@@ -15414,7 +15461,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="291" spans="1:15">
+    <row r="291" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>553</v>
       </c>
@@ -15455,7 +15502,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="292" spans="1:15">
+    <row r="292" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>553</v>
       </c>
@@ -15502,7 +15549,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="293" spans="1:15">
+    <row r="293" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>557</v>
       </c>
@@ -15543,7 +15590,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="294" spans="1:15">
+    <row r="294" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>557</v>
       </c>
@@ -15590,7 +15637,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="295" spans="1:15">
+    <row r="295" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>560</v>
       </c>
@@ -15631,7 +15678,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="296" spans="1:15">
+    <row r="296" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>560</v>
       </c>
@@ -15678,7 +15725,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="297" spans="1:15">
+    <row r="297" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>560</v>
       </c>
@@ -15725,7 +15772,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="298" spans="1:15">
+    <row r="298" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>564</v>
       </c>
@@ -15766,7 +15813,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="299" spans="1:15">
+    <row r="299" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>564</v>
       </c>
@@ -15813,7 +15860,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="300" spans="1:15">
+    <row r="300" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>568</v>
       </c>
@@ -15854,7 +15901,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="301" spans="1:15">
+    <row r="301" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>568</v>
       </c>
@@ -15901,7 +15948,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="302" spans="1:15">
+    <row r="302" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>568</v>
       </c>
@@ -15948,7 +15995,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="303" spans="1:15">
+    <row r="303" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>573</v>
       </c>
@@ -15989,7 +16036,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="304" spans="1:15">
+    <row r="304" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>573</v>
       </c>
@@ -16036,7 +16083,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="305" spans="1:15">
+    <row r="305" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>573</v>
       </c>
@@ -16083,7 +16130,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="306" spans="1:15">
+    <row r="306" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>573</v>
       </c>
@@ -16130,7 +16177,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="307" spans="1:15">
+    <row r="307" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>573</v>
       </c>
@@ -16177,7 +16224,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="308" spans="1:15">
+    <row r="308" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>573</v>
       </c>
@@ -16224,7 +16271,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="309" spans="1:15">
+    <row r="309" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>573</v>
       </c>
@@ -16271,7 +16318,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="310" spans="1:15">
+    <row r="310" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>573</v>
       </c>
@@ -16318,7 +16365,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="311" spans="1:15">
+    <row r="311" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>573</v>
       </c>
@@ -16365,7 +16412,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="312" spans="1:15">
+    <row r="312" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>573</v>
       </c>
@@ -16412,7 +16459,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="313" spans="1:15">
+    <row r="313" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>587</v>
       </c>
@@ -16453,7 +16500,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="314" spans="1:15">
+    <row r="314" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>587</v>
       </c>
@@ -16500,7 +16547,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="315" spans="1:15">
+    <row r="315" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>587</v>
       </c>
@@ -16547,7 +16594,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="316" spans="1:15">
+    <row r="316" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>587</v>
       </c>
@@ -16594,7 +16641,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="317" spans="1:15">
+    <row r="317" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>587</v>
       </c>
@@ -16641,7 +16688,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="318" spans="1:15">
+    <row r="318" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>595</v>
       </c>
@@ -16682,7 +16729,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="319" spans="1:15">
+    <row r="319" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>595</v>
       </c>
@@ -16729,7 +16776,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="320" spans="1:15">
+    <row r="320" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>599</v>
       </c>
@@ -16770,7 +16817,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="321" spans="1:15">
+    <row r="321" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>601</v>
       </c>
@@ -16811,7 +16858,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="322" spans="1:15">
+    <row r="322" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>601</v>
       </c>
@@ -16858,7 +16905,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="323" spans="1:15">
+    <row r="323" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>601</v>
       </c>
@@ -16905,7 +16952,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="324" spans="1:15">
+    <row r="324" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>601</v>
       </c>
@@ -16952,7 +16999,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="325" spans="1:15">
+    <row r="325" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>601</v>
       </c>
@@ -16999,7 +17046,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="326" spans="1:15">
+    <row r="326" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>601</v>
       </c>
@@ -17046,7 +17093,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="327" spans="1:15">
+    <row r="327" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>601</v>
       </c>
@@ -17093,7 +17140,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="328" spans="1:15">
+    <row r="328" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>601</v>
       </c>
@@ -17140,7 +17187,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="329" spans="1:15">
+    <row r="329" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>601</v>
       </c>
@@ -17187,7 +17234,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="330" spans="1:15">
+    <row r="330" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>601</v>
       </c>
@@ -17234,7 +17281,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="331" spans="1:15">
+    <row r="331" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>621</v>
       </c>
@@ -17275,7 +17322,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="332" spans="1:15">
+    <row r="332" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>621</v>
       </c>
@@ -17322,7 +17369,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="333" spans="1:15">
+    <row r="333" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>621</v>
       </c>
@@ -17369,7 +17416,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="334" spans="1:15">
+    <row r="334" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>621</v>
       </c>
@@ -17416,7 +17463,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="335" spans="1:15">
+    <row r="335" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>621</v>
       </c>
@@ -17463,7 +17510,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="336" spans="1:15">
+    <row r="336" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>621</v>
       </c>
@@ -17510,7 +17557,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="337" spans="1:15">
+    <row r="337" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>632</v>
       </c>
@@ -17551,7 +17598,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="338" spans="1:15">
+    <row r="338" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>632</v>
       </c>
@@ -17598,7 +17645,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="339" spans="1:15">
+    <row r="339" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>635</v>
       </c>
@@ -17639,7 +17686,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="340" spans="1:15">
+    <row r="340" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>635</v>
       </c>
@@ -17686,7 +17733,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="341" spans="1:15">
+    <row r="341" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>635</v>
       </c>
@@ -17733,7 +17780,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="342" spans="1:15">
+    <row r="342" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>641</v>
       </c>
@@ -17774,7 +17821,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="343" spans="1:15">
+    <row r="343" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>644</v>
       </c>
@@ -17815,7 +17862,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="344" spans="1:15">
+    <row r="344" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>647</v>
       </c>
@@ -17856,7 +17903,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="345" spans="1:15">
+    <row r="345" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>647</v>
       </c>
@@ -17903,7 +17950,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="346" spans="1:15">
+    <row r="346" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>647</v>
       </c>
@@ -17950,7 +17997,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="347" spans="1:15">
+    <row r="347" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>647</v>
       </c>
@@ -17997,7 +18044,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="348" spans="1:15">
+    <row r="348" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>652</v>
       </c>
@@ -18038,7 +18085,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="349" spans="1:15">
+    <row r="349" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>654</v>
       </c>
@@ -18079,7 +18126,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="350" spans="1:15">
+    <row r="350" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>657</v>
       </c>
@@ -18120,7 +18167,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="351" spans="1:15">
+    <row r="351" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>660</v>
       </c>
@@ -18161,7 +18208,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="352" spans="1:15">
+    <row r="352" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>660</v>
       </c>
@@ -18208,7 +18255,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="353" spans="1:15">
+    <row r="353" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>660</v>
       </c>
@@ -18255,7 +18302,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="354" spans="1:15">
+    <row r="354" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>660</v>
       </c>
@@ -18302,7 +18349,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="355" spans="1:15">
+    <row r="355" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>665</v>
       </c>
@@ -18343,7 +18390,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="356" spans="1:15">
+    <row r="356" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>665</v>
       </c>
@@ -18390,7 +18437,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="357" spans="1:15">
+    <row r="357" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>665</v>
       </c>
@@ -18437,7 +18484,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="358" spans="1:15">
+    <row r="358" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>669</v>
       </c>
@@ -18478,7 +18525,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="359" spans="1:15">
+    <row r="359" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>669</v>
       </c>
@@ -18525,7 +18572,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="360" spans="1:15">
+    <row r="360" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>672</v>
       </c>
@@ -18566,7 +18613,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="361" spans="1:15">
+    <row r="361" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>672</v>
       </c>
@@ -18613,7 +18660,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="362" spans="1:15">
+    <row r="362" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>676</v>
       </c>
@@ -18655,7 +18702,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P362"/>
+  <autoFilter ref="A1:P362" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor edits to script 01-04. Added some Rhat and ess summaries and trace plots to 04_run_dabom.R
</commit_message>
<xml_diff>
--- a/outgoing/PITcleanr/PRO_Steelhead_2019.xlsx
+++ b/outgoing/PITcleanr/PRO_Steelhead_2019.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seek/Documents/GitProjects/MyProjects/DabomYakimaSthd/outgoing/PITcleanr/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE110E2-6FE2-6241-88F3-089250D6A9BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25180" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="ProcCapHist" sheetId="1" r:id="rId1"/>
@@ -18,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ProcCapHist!$A$1:$P$362</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -2065,8 +2059,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2112,14 +2106,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -2166,7 +2152,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2198,27 +2184,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2250,24 +2218,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2443,34 +2393,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P362"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N1" sqref="N1:O1048576"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="4" width="21.5" customWidth="1"/>
-    <col min="5" max="5" width="10.5" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" customWidth="1"/>
-    <col min="8" max="8" width="9.5" customWidth="1"/>
-    <col min="9" max="10" width="10.5" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" customWidth="1"/>
-    <col min="12" max="13" width="16.1640625" customWidth="1"/>
-    <col min="14" max="14" width="9.5" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2520,7 +2473,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -2561,7 +2514,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2608,7 +2561,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2655,7 +2608,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2702,7 +2655,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2749,7 +2702,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2796,7 +2749,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -2843,7 +2796,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -2884,7 +2837,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -2931,7 +2884,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -2978,7 +2931,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -3019,7 +2972,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -3066,7 +3019,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -3113,7 +3066,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -3160,7 +3113,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -3207,7 +3160,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -3254,7 +3207,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -3295,7 +3248,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -3336,7 +3289,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -3383,7 +3336,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>70</v>
       </c>
@@ -3430,7 +3383,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -3471,7 +3424,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -3518,7 +3471,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>80</v>
       </c>
@@ -3565,7 +3518,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -3606,7 +3559,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -3647,7 +3600,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
         <v>88</v>
       </c>
@@ -3694,7 +3647,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -3735,7 +3688,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
         <v>93</v>
       </c>
@@ -3782,7 +3735,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
         <v>93</v>
       </c>
@@ -3829,7 +3782,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15">
       <c r="A31" t="s">
         <v>93</v>
       </c>
@@ -3876,7 +3829,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15">
       <c r="A32" t="s">
         <v>103</v>
       </c>
@@ -3917,7 +3870,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>103</v>
       </c>
@@ -3964,7 +3917,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
         <v>108</v>
       </c>
@@ -4005,7 +3958,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>108</v>
       </c>
@@ -4052,7 +4005,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
         <v>108</v>
       </c>
@@ -4099,7 +4052,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
         <v>108</v>
       </c>
@@ -4146,7 +4099,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
         <v>108</v>
       </c>
@@ -4193,7 +4146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>116</v>
       </c>
@@ -4234,7 +4187,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>116</v>
       </c>
@@ -4281,7 +4234,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>116</v>
       </c>
@@ -4328,7 +4281,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
         <v>122</v>
       </c>
@@ -4369,7 +4322,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
         <v>122</v>
       </c>
@@ -4416,7 +4369,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15">
       <c r="A44" t="s">
         <v>122</v>
       </c>
@@ -4463,7 +4416,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15">
       <c r="A45" t="s">
         <v>122</v>
       </c>
@@ -4510,7 +4463,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15">
       <c r="A46" t="s">
         <v>122</v>
       </c>
@@ -4551,7 +4504,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
         <v>130</v>
       </c>
@@ -4592,7 +4545,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
         <v>133</v>
       </c>
@@ -4633,7 +4586,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15">
       <c r="A49" t="s">
         <v>133</v>
       </c>
@@ -4680,7 +4633,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15">
       <c r="A50" t="s">
         <v>137</v>
       </c>
@@ -4721,7 +4674,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15">
       <c r="A51" t="s">
         <v>137</v>
       </c>
@@ -4768,7 +4721,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15">
       <c r="A52" t="s">
         <v>137</v>
       </c>
@@ -4815,7 +4768,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15">
       <c r="A53" t="s">
         <v>141</v>
       </c>
@@ -4856,7 +4809,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15">
       <c r="A54" t="s">
         <v>141</v>
       </c>
@@ -4903,7 +4856,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15">
       <c r="A55" t="s">
         <v>141</v>
       </c>
@@ -4950,7 +4903,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15">
       <c r="A56" t="s">
         <v>147</v>
       </c>
@@ -4991,7 +4944,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15">
       <c r="A57" t="s">
         <v>147</v>
       </c>
@@ -5038,7 +4991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15">
       <c r="A58" t="s">
         <v>147</v>
       </c>
@@ -5085,7 +5038,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15">
       <c r="A59" t="s">
         <v>147</v>
       </c>
@@ -5126,7 +5079,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15">
       <c r="A60" t="s">
         <v>152</v>
       </c>
@@ -5167,7 +5120,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15">
       <c r="A61" t="s">
         <v>152</v>
       </c>
@@ -5214,7 +5167,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15">
       <c r="A62" t="s">
         <v>152</v>
       </c>
@@ -5261,7 +5214,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15">
       <c r="A63" t="s">
         <v>160</v>
       </c>
@@ -5302,7 +5255,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15">
       <c r="A64" t="s">
         <v>160</v>
       </c>
@@ -5349,7 +5302,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15">
       <c r="A65" t="s">
         <v>160</v>
       </c>
@@ -5396,7 +5349,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15">
       <c r="A66" t="s">
         <v>166</v>
       </c>
@@ -5437,7 +5390,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15">
       <c r="A67" t="s">
         <v>166</v>
       </c>
@@ -5484,7 +5437,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15">
       <c r="A68" t="s">
         <v>166</v>
       </c>
@@ -5531,7 +5484,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15">
       <c r="A69" t="s">
         <v>166</v>
       </c>
@@ -5578,7 +5531,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:15">
       <c r="A70" t="s">
         <v>166</v>
       </c>
@@ -5625,7 +5578,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:15">
       <c r="A71" t="s">
         <v>174</v>
       </c>
@@ -5666,7 +5619,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:15">
       <c r="A72" t="s">
         <v>174</v>
       </c>
@@ -5713,7 +5666,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15">
       <c r="A73" t="s">
         <v>179</v>
       </c>
@@ -5754,7 +5707,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:15">
       <c r="A74" t="s">
         <v>179</v>
       </c>
@@ -5801,7 +5754,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:15">
       <c r="A75" t="s">
         <v>185</v>
       </c>
@@ -5842,7 +5795,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:15">
       <c r="A76" t="s">
         <v>185</v>
       </c>
@@ -5889,7 +5842,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:15">
       <c r="A77" t="s">
         <v>185</v>
       </c>
@@ -5936,7 +5889,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:15">
       <c r="A78" t="s">
         <v>185</v>
       </c>
@@ -5983,7 +5936,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:15">
       <c r="A79" t="s">
         <v>185</v>
       </c>
@@ -6030,7 +5983,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:15">
       <c r="A80" t="s">
         <v>192</v>
       </c>
@@ -6071,7 +6024,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:15">
       <c r="A81" t="s">
         <v>192</v>
       </c>
@@ -6118,7 +6071,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:15">
       <c r="A82" t="s">
         <v>192</v>
       </c>
@@ -6159,7 +6112,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:15">
       <c r="A83" t="s">
         <v>197</v>
       </c>
@@ -6200,7 +6153,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:15">
       <c r="A84" t="s">
         <v>200</v>
       </c>
@@ -6241,7 +6194,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:15">
       <c r="A85" t="s">
         <v>200</v>
       </c>
@@ -6288,7 +6241,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:15">
       <c r="A86" t="s">
         <v>200</v>
       </c>
@@ -6335,7 +6288,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:15">
       <c r="A87" t="s">
         <v>200</v>
       </c>
@@ -6376,7 +6329,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:15">
       <c r="A88" t="s">
         <v>207</v>
       </c>
@@ -6417,7 +6370,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:15">
       <c r="A89" t="s">
         <v>209</v>
       </c>
@@ -6458,7 +6411,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:15">
       <c r="A90" t="s">
         <v>209</v>
       </c>
@@ -6505,7 +6458,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:15">
       <c r="A91" t="s">
         <v>209</v>
       </c>
@@ -6552,7 +6505,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:15">
       <c r="A92" t="s">
         <v>209</v>
       </c>
@@ -6593,7 +6546,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:15">
       <c r="A93" t="s">
         <v>216</v>
       </c>
@@ -6634,7 +6587,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:15">
       <c r="A94" t="s">
         <v>216</v>
       </c>
@@ -6681,7 +6634,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:15">
       <c r="A95" t="s">
         <v>216</v>
       </c>
@@ -6728,7 +6681,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:15">
       <c r="A96" t="s">
         <v>216</v>
       </c>
@@ -6775,7 +6728,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:15">
       <c r="A97" t="s">
         <v>216</v>
       </c>
@@ -6816,7 +6769,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:15">
       <c r="A98" t="s">
         <v>224</v>
       </c>
@@ -6857,7 +6810,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:15">
       <c r="A99" t="s">
         <v>224</v>
       </c>
@@ -6904,7 +6857,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:15">
       <c r="A100" t="s">
         <v>224</v>
       </c>
@@ -6951,7 +6904,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:15">
       <c r="A101" t="s">
         <v>224</v>
       </c>
@@ -6998,7 +6951,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:15">
       <c r="A102" t="s">
         <v>224</v>
       </c>
@@ -7045,7 +6998,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:15">
       <c r="A103" t="s">
         <v>224</v>
       </c>
@@ -7092,7 +7045,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:15">
       <c r="A104" t="s">
         <v>224</v>
       </c>
@@ -7139,7 +7092,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:15">
       <c r="A105" t="s">
         <v>233</v>
       </c>
@@ -7180,7 +7133,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:15">
       <c r="A106" t="s">
         <v>237</v>
       </c>
@@ -7221,7 +7174,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:15">
       <c r="A107" t="s">
         <v>237</v>
       </c>
@@ -7268,7 +7221,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:15">
       <c r="A108" t="s">
         <v>237</v>
       </c>
@@ -7315,7 +7268,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:15">
       <c r="A109" t="s">
         <v>237</v>
       </c>
@@ -7362,7 +7315,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:15">
       <c r="A110" t="s">
         <v>237</v>
       </c>
@@ -7409,7 +7362,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:15">
       <c r="A111" t="s">
         <v>237</v>
       </c>
@@ -7456,7 +7409,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:15">
       <c r="A112" t="s">
         <v>237</v>
       </c>
@@ -7503,7 +7456,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:15">
       <c r="A113" t="s">
         <v>237</v>
       </c>
@@ -7550,7 +7503,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:15">
       <c r="A114" t="s">
         <v>237</v>
       </c>
@@ -7597,7 +7550,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:15">
       <c r="A115" t="s">
         <v>237</v>
       </c>
@@ -7644,7 +7597,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:15">
       <c r="A116" t="s">
         <v>237</v>
       </c>
@@ -7691,7 +7644,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:15">
       <c r="A117" t="s">
         <v>237</v>
       </c>
@@ -7738,7 +7691,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:15">
       <c r="A118" t="s">
         <v>237</v>
       </c>
@@ -7785,7 +7738,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:15">
       <c r="A119" t="s">
         <v>237</v>
       </c>
@@ -7832,7 +7785,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:15">
       <c r="A120" t="s">
         <v>259</v>
       </c>
@@ -7873,7 +7826,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:15">
       <c r="A121" t="s">
         <v>259</v>
       </c>
@@ -7920,7 +7873,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:15">
       <c r="A122" t="s">
         <v>259</v>
       </c>
@@ -7967,7 +7920,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:15">
       <c r="A123" t="s">
         <v>259</v>
       </c>
@@ -8014,7 +7967,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:15">
       <c r="A124" t="s">
         <v>265</v>
       </c>
@@ -8055,7 +8008,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:15">
       <c r="A125" t="s">
         <v>265</v>
       </c>
@@ -8102,7 +8055,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:15">
       <c r="A126" t="s">
         <v>265</v>
       </c>
@@ -8149,7 +8102,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:15">
       <c r="A127" t="s">
         <v>265</v>
       </c>
@@ -8196,7 +8149,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:15">
       <c r="A128" t="s">
         <v>265</v>
       </c>
@@ -8243,7 +8196,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:15">
       <c r="A129" t="s">
         <v>271</v>
       </c>
@@ -8284,7 +8237,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:15">
       <c r="A130" t="s">
         <v>271</v>
       </c>
@@ -8331,7 +8284,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:15">
       <c r="A131" t="s">
         <v>271</v>
       </c>
@@ -8378,7 +8331,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:15">
       <c r="A132" t="s">
         <v>276</v>
       </c>
@@ -8419,7 +8372,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:15">
       <c r="A133" t="s">
         <v>276</v>
       </c>
@@ -8466,7 +8419,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:15">
       <c r="A134" t="s">
         <v>276</v>
       </c>
@@ -8513,7 +8466,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:15">
       <c r="A135" t="s">
         <v>276</v>
       </c>
@@ -8560,7 +8513,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:15">
       <c r="A136" t="s">
         <v>281</v>
       </c>
@@ -8601,7 +8554,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:15">
       <c r="A137" t="s">
         <v>281</v>
       </c>
@@ -8648,7 +8601,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:15">
       <c r="A138" t="s">
         <v>281</v>
       </c>
@@ -8695,7 +8648,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:15">
       <c r="A139" t="s">
         <v>286</v>
       </c>
@@ -8736,7 +8689,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:15">
       <c r="A140" t="s">
         <v>286</v>
       </c>
@@ -8783,7 +8736,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:15">
       <c r="A141" t="s">
         <v>286</v>
       </c>
@@ -8824,7 +8777,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:15">
       <c r="A142" t="s">
         <v>291</v>
       </c>
@@ -8865,7 +8818,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:15">
       <c r="A143" t="s">
         <v>291</v>
       </c>
@@ -8912,7 +8865,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:15">
       <c r="A144" t="s">
         <v>291</v>
       </c>
@@ -8959,7 +8912,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:15">
       <c r="A145" t="s">
         <v>291</v>
       </c>
@@ -9006,7 +8959,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:15">
       <c r="A146" t="s">
         <v>291</v>
       </c>
@@ -9053,7 +9006,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:15">
       <c r="A147" t="s">
         <v>298</v>
       </c>
@@ -9094,7 +9047,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:15">
       <c r="A148" t="s">
         <v>298</v>
       </c>
@@ -9141,7 +9094,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:15">
       <c r="A149" t="s">
         <v>298</v>
       </c>
@@ -9188,7 +9141,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:15">
       <c r="A150" t="s">
         <v>298</v>
       </c>
@@ -9235,7 +9188,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:15">
       <c r="A151" t="s">
         <v>298</v>
       </c>
@@ -9282,7 +9235,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:15">
       <c r="A152" t="s">
         <v>309</v>
       </c>
@@ -9323,7 +9276,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:15">
       <c r="A153" t="s">
         <v>309</v>
       </c>
@@ -9370,7 +9323,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:15">
       <c r="A154" t="s">
         <v>312</v>
       </c>
@@ -9411,7 +9364,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:15">
       <c r="A155" t="s">
         <v>312</v>
       </c>
@@ -9458,7 +9411,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:15">
       <c r="A156" t="s">
         <v>312</v>
       </c>
@@ -9505,7 +9458,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:15">
       <c r="A157" t="s">
         <v>312</v>
       </c>
@@ -9552,7 +9505,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:15">
       <c r="A158" t="s">
         <v>318</v>
       </c>
@@ -9593,7 +9546,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:15">
       <c r="A159" t="s">
         <v>322</v>
       </c>
@@ -9634,7 +9587,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:15">
       <c r="A160" t="s">
         <v>322</v>
       </c>
@@ -9681,7 +9634,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:15">
       <c r="A161" t="s">
         <v>322</v>
       </c>
@@ -9728,7 +9681,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:15">
       <c r="A162" t="s">
         <v>322</v>
       </c>
@@ -9775,7 +9728,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:15">
       <c r="A163" t="s">
         <v>322</v>
       </c>
@@ -9822,7 +9775,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:15">
       <c r="A164" t="s">
         <v>331</v>
       </c>
@@ -9863,7 +9816,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:15">
       <c r="A165" t="s">
         <v>334</v>
       </c>
@@ -9904,7 +9857,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:15">
       <c r="A166" t="s">
         <v>334</v>
       </c>
@@ -9951,7 +9904,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:15">
       <c r="A167" t="s">
         <v>338</v>
       </c>
@@ -9992,7 +9945,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:15">
       <c r="A168" t="s">
         <v>338</v>
       </c>
@@ -10039,7 +9992,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:15">
       <c r="A169" t="s">
         <v>338</v>
       </c>
@@ -10086,7 +10039,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:15">
       <c r="A170" t="s">
         <v>343</v>
       </c>
@@ -10121,7 +10074,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:15">
       <c r="A171" t="s">
         <v>343</v>
       </c>
@@ -10162,7 +10115,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:15">
       <c r="A172" t="s">
         <v>343</v>
       </c>
@@ -10200,7 +10153,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:15">
       <c r="A173" t="s">
         <v>343</v>
       </c>
@@ -10241,7 +10194,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:15">
       <c r="A174" t="s">
         <v>343</v>
       </c>
@@ -10282,7 +10235,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:15">
       <c r="A175" t="s">
         <v>350</v>
       </c>
@@ -10323,7 +10276,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:15">
       <c r="A176" t="s">
         <v>350</v>
       </c>
@@ -10370,7 +10323,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:15">
       <c r="A177" t="s">
         <v>350</v>
       </c>
@@ -10417,7 +10370,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:15">
       <c r="A178" t="s">
         <v>350</v>
       </c>
@@ -10464,7 +10417,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:15">
       <c r="A179" t="s">
         <v>350</v>
       </c>
@@ -10511,7 +10464,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:15">
       <c r="A180" t="s">
         <v>350</v>
       </c>
@@ -10558,7 +10511,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:15">
       <c r="A181" t="s">
         <v>350</v>
       </c>
@@ -10605,7 +10558,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:15">
       <c r="A182" t="s">
         <v>350</v>
       </c>
@@ -10652,7 +10605,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:15">
       <c r="A183" t="s">
         <v>350</v>
       </c>
@@ -10699,7 +10652,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:15">
       <c r="A184" t="s">
         <v>350</v>
       </c>
@@ -10746,7 +10699,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:15">
       <c r="A185" t="s">
         <v>350</v>
       </c>
@@ -10793,7 +10746,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:15">
       <c r="A186" t="s">
         <v>350</v>
       </c>
@@ -10840,7 +10793,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:15">
       <c r="A187" t="s">
         <v>350</v>
       </c>
@@ -10887,7 +10840,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:15">
       <c r="A188" t="s">
         <v>350</v>
       </c>
@@ -10934,7 +10887,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:15">
       <c r="A189" t="s">
         <v>350</v>
       </c>
@@ -10981,7 +10934,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:15">
       <c r="A190" t="s">
         <v>350</v>
       </c>
@@ -11028,7 +10981,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:15">
       <c r="A191" t="s">
         <v>350</v>
       </c>
@@ -11075,7 +11028,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:15">
       <c r="A192" t="s">
         <v>350</v>
       </c>
@@ -11122,7 +11075,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:15">
       <c r="A193" t="s">
         <v>388</v>
       </c>
@@ -11163,7 +11116,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:15">
       <c r="A194" t="s">
         <v>392</v>
       </c>
@@ -11204,7 +11157,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:15">
       <c r="A195" t="s">
         <v>392</v>
       </c>
@@ -11251,7 +11204,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:15">
       <c r="A196" t="s">
         <v>392</v>
       </c>
@@ -11298,7 +11251,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:15">
       <c r="A197" t="s">
         <v>392</v>
       </c>
@@ -11345,7 +11298,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:15">
       <c r="A198" t="s">
         <v>392</v>
       </c>
@@ -11392,7 +11345,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:15">
       <c r="A199" t="s">
         <v>398</v>
       </c>
@@ -11433,7 +11386,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:15">
       <c r="A200" t="s">
         <v>398</v>
       </c>
@@ -11480,7 +11433,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:15">
       <c r="A201" t="s">
         <v>398</v>
       </c>
@@ -11527,7 +11480,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:15">
       <c r="A202" t="s">
         <v>398</v>
       </c>
@@ -11574,7 +11527,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:15">
       <c r="A203" t="s">
         <v>398</v>
       </c>
@@ -11621,7 +11574,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:15">
       <c r="A204" t="s">
         <v>398</v>
       </c>
@@ -11668,7 +11621,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:15">
       <c r="A205" t="s">
         <v>398</v>
       </c>
@@ -11715,7 +11668,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:15">
       <c r="A206" t="s">
         <v>407</v>
       </c>
@@ -11750,7 +11703,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:15">
       <c r="A207" t="s">
         <v>407</v>
       </c>
@@ -11791,7 +11744,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:15">
       <c r="A208" t="s">
         <v>407</v>
       </c>
@@ -11829,7 +11782,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:15">
       <c r="A209" t="s">
         <v>407</v>
       </c>
@@ -11870,7 +11823,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:15">
       <c r="A210" t="s">
         <v>421</v>
       </c>
@@ -11911,7 +11864,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:15">
       <c r="A211" t="s">
         <v>421</v>
       </c>
@@ -11958,7 +11911,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:15">
       <c r="A212" t="s">
         <v>421</v>
       </c>
@@ -12005,7 +11958,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:15">
       <c r="A213" t="s">
         <v>421</v>
       </c>
@@ -12052,7 +12005,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="214" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:15">
       <c r="A214" t="s">
         <v>421</v>
       </c>
@@ -12099,7 +12052,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:15">
       <c r="A215" t="s">
         <v>421</v>
       </c>
@@ -12146,7 +12099,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:15">
       <c r="A216" t="s">
         <v>429</v>
       </c>
@@ -12187,7 +12140,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:15">
       <c r="A217" t="s">
         <v>429</v>
       </c>
@@ -12234,7 +12187,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="218" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:15">
       <c r="A218" t="s">
         <v>433</v>
       </c>
@@ -12275,7 +12228,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:15">
       <c r="A219" t="s">
         <v>433</v>
       </c>
@@ -12322,7 +12275,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="220" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:15">
       <c r="A220" t="s">
         <v>436</v>
       </c>
@@ -12363,7 +12316,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="221" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:15">
       <c r="A221" t="s">
         <v>436</v>
       </c>
@@ -12410,7 +12363,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="222" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:15">
       <c r="A222" t="s">
         <v>436</v>
       </c>
@@ -12457,7 +12410,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="223" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:15">
       <c r="A223" t="s">
         <v>436</v>
       </c>
@@ -12504,7 +12457,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:15">
       <c r="A224" t="s">
         <v>436</v>
       </c>
@@ -12551,7 +12504,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="225" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:15">
       <c r="A225" t="s">
         <v>436</v>
       </c>
@@ -12598,7 +12551,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:15">
       <c r="A226" t="s">
         <v>449</v>
       </c>
@@ -12639,7 +12592,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="227" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:15">
       <c r="A227" t="s">
         <v>449</v>
       </c>
@@ -12686,7 +12639,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="228" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:15">
       <c r="A228" t="s">
         <v>452</v>
       </c>
@@ -12727,7 +12680,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="229" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:15">
       <c r="A229" t="s">
         <v>452</v>
       </c>
@@ -12774,7 +12727,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="230" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:15">
       <c r="A230" t="s">
         <v>452</v>
       </c>
@@ -12815,7 +12768,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="231" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:15">
       <c r="A231" t="s">
         <v>456</v>
       </c>
@@ -12856,7 +12809,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="232" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:15">
       <c r="A232" t="s">
         <v>456</v>
       </c>
@@ -12903,7 +12856,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="233" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:15">
       <c r="A233" t="s">
         <v>456</v>
       </c>
@@ -12950,7 +12903,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="234" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:15">
       <c r="A234" t="s">
         <v>462</v>
       </c>
@@ -12991,7 +12944,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="235" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:15">
       <c r="A235" t="s">
         <v>462</v>
       </c>
@@ -13038,7 +12991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="236" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:15">
       <c r="A236" t="s">
         <v>465</v>
       </c>
@@ -13079,7 +13032,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="237" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:15">
       <c r="A237" t="s">
         <v>465</v>
       </c>
@@ -13126,7 +13079,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="238" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:15">
       <c r="A238" t="s">
         <v>465</v>
       </c>
@@ -13173,7 +13126,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="239" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:15">
       <c r="A239" t="s">
         <v>465</v>
       </c>
@@ -13220,7 +13173,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="240" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:15">
       <c r="A240" t="s">
         <v>471</v>
       </c>
@@ -13261,7 +13214,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="241" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:15">
       <c r="A241" t="s">
         <v>471</v>
       </c>
@@ -13308,7 +13261,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="242" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:15">
       <c r="A242" t="s">
         <v>474</v>
       </c>
@@ -13349,7 +13302,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="243" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:15">
       <c r="A243" t="s">
         <v>474</v>
       </c>
@@ -13396,7 +13349,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="244" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:15">
       <c r="A244" t="s">
         <v>474</v>
       </c>
@@ -13443,7 +13396,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="245" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:15">
       <c r="A245" t="s">
         <v>474</v>
       </c>
@@ -13490,7 +13443,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="246" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:15">
       <c r="A246" t="s">
         <v>481</v>
       </c>
@@ -13531,7 +13484,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="247" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:15">
       <c r="A247" t="s">
         <v>481</v>
       </c>
@@ -13578,7 +13531,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="248" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:15">
       <c r="A248" t="s">
         <v>481</v>
       </c>
@@ -13619,7 +13572,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="249" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:15">
       <c r="A249" t="s">
         <v>485</v>
       </c>
@@ -13660,7 +13613,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="250" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:15">
       <c r="A250" t="s">
         <v>488</v>
       </c>
@@ -13701,7 +13654,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="251" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:15">
       <c r="A251" t="s">
         <v>488</v>
       </c>
@@ -13748,7 +13701,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="252" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:15">
       <c r="A252" t="s">
         <v>488</v>
       </c>
@@ -13795,7 +13748,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="253" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:15">
       <c r="A253" t="s">
         <v>492</v>
       </c>
@@ -13836,7 +13789,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="254" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:15">
       <c r="A254" t="s">
         <v>492</v>
       </c>
@@ -13883,7 +13836,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="255" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:15">
       <c r="A255" t="s">
         <v>495</v>
       </c>
@@ -13924,7 +13877,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="256" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:15">
       <c r="A256" t="s">
         <v>495</v>
       </c>
@@ -13971,7 +13924,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="257" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:15">
       <c r="A257" t="s">
         <v>495</v>
       </c>
@@ -14012,7 +13965,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="258" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:15">
       <c r="A258" t="s">
         <v>499</v>
       </c>
@@ -14053,7 +14006,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="259" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:15">
       <c r="A259" t="s">
         <v>499</v>
       </c>
@@ -14100,7 +14053,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="260" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:15">
       <c r="A260" t="s">
         <v>499</v>
       </c>
@@ -14141,7 +14094,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="261" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:15">
       <c r="A261" t="s">
         <v>504</v>
       </c>
@@ -14182,7 +14135,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="262" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:15">
       <c r="A262" t="s">
         <v>506</v>
       </c>
@@ -14223,7 +14176,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="263" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:15">
       <c r="A263" t="s">
         <v>506</v>
       </c>
@@ -14270,7 +14223,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="264" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:15">
       <c r="A264" t="s">
         <v>506</v>
       </c>
@@ -14317,7 +14270,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="265" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:15">
       <c r="A265" t="s">
         <v>510</v>
       </c>
@@ -14358,7 +14311,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="266" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:15">
       <c r="A266" t="s">
         <v>510</v>
       </c>
@@ -14405,7 +14358,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="267" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:15">
       <c r="A267" t="s">
         <v>510</v>
       </c>
@@ -14452,7 +14405,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="268" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:15">
       <c r="A268" t="s">
         <v>515</v>
       </c>
@@ -14493,7 +14446,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="269" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:15">
       <c r="A269" t="s">
         <v>515</v>
       </c>
@@ -14540,7 +14493,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="270" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:15">
       <c r="A270" t="s">
         <v>518</v>
       </c>
@@ -14581,7 +14534,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="271" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:15">
       <c r="A271" t="s">
         <v>520</v>
       </c>
@@ -14622,7 +14575,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="272" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:15">
       <c r="A272" t="s">
         <v>520</v>
       </c>
@@ -14669,7 +14622,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="273" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:15">
       <c r="A273" t="s">
         <v>524</v>
       </c>
@@ -14710,7 +14663,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="274" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:15">
       <c r="A274" t="s">
         <v>527</v>
       </c>
@@ -14751,7 +14704,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="275" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:15">
       <c r="A275" t="s">
         <v>527</v>
       </c>
@@ -14798,7 +14751,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="276" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:15">
       <c r="A276" t="s">
         <v>527</v>
       </c>
@@ -14845,7 +14798,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="277" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:15">
       <c r="A277" t="s">
         <v>531</v>
       </c>
@@ -14886,7 +14839,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="278" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:15">
       <c r="A278" t="s">
         <v>534</v>
       </c>
@@ -14927,7 +14880,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="279" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:15">
       <c r="A279" t="s">
         <v>534</v>
       </c>
@@ -14974,7 +14927,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="280" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:15">
       <c r="A280" t="s">
         <v>538</v>
       </c>
@@ -15015,7 +14968,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="281" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:15">
       <c r="A281" t="s">
         <v>538</v>
       </c>
@@ -15062,7 +15015,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="282" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:15">
       <c r="A282" t="s">
         <v>538</v>
       </c>
@@ -15103,7 +15056,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="283" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:15">
       <c r="A283" t="s">
         <v>543</v>
       </c>
@@ -15144,7 +15097,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="284" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:15">
       <c r="A284" t="s">
         <v>543</v>
       </c>
@@ -15191,7 +15144,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="285" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:15">
       <c r="A285" t="s">
         <v>543</v>
       </c>
@@ -15238,7 +15191,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="286" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:15">
       <c r="A286" t="s">
         <v>543</v>
       </c>
@@ -15285,7 +15238,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="287" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:15">
       <c r="A287" t="s">
         <v>549</v>
       </c>
@@ -15326,7 +15279,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="288" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:15">
       <c r="A288" t="s">
         <v>549</v>
       </c>
@@ -15373,7 +15326,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="289" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:15">
       <c r="A289" t="s">
         <v>549</v>
       </c>
@@ -15420,7 +15373,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="290" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:15">
       <c r="A290" t="s">
         <v>549</v>
       </c>
@@ -15461,7 +15414,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="291" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:15">
       <c r="A291" t="s">
         <v>553</v>
       </c>
@@ -15502,7 +15455,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="292" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:15">
       <c r="A292" t="s">
         <v>553</v>
       </c>
@@ -15549,7 +15502,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="293" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:15">
       <c r="A293" t="s">
         <v>557</v>
       </c>
@@ -15590,7 +15543,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="294" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:15">
       <c r="A294" t="s">
         <v>557</v>
       </c>
@@ -15637,7 +15590,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="295" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:15">
       <c r="A295" t="s">
         <v>560</v>
       </c>
@@ -15678,7 +15631,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="296" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:15">
       <c r="A296" t="s">
         <v>560</v>
       </c>
@@ -15725,7 +15678,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="297" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:15">
       <c r="A297" t="s">
         <v>560</v>
       </c>
@@ -15772,7 +15725,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="298" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:15">
       <c r="A298" t="s">
         <v>564</v>
       </c>
@@ -15813,7 +15766,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="299" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:15">
       <c r="A299" t="s">
         <v>564</v>
       </c>
@@ -15860,7 +15813,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="300" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:15">
       <c r="A300" t="s">
         <v>568</v>
       </c>
@@ -15901,7 +15854,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="301" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:15">
       <c r="A301" t="s">
         <v>568</v>
       </c>
@@ -15948,7 +15901,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="302" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:15">
       <c r="A302" t="s">
         <v>568</v>
       </c>
@@ -15995,7 +15948,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="303" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:15">
       <c r="A303" t="s">
         <v>573</v>
       </c>
@@ -16036,7 +15989,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="304" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:15">
       <c r="A304" t="s">
         <v>573</v>
       </c>
@@ -16083,7 +16036,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="305" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:15">
       <c r="A305" t="s">
         <v>573</v>
       </c>
@@ -16130,7 +16083,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="306" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:15">
       <c r="A306" t="s">
         <v>573</v>
       </c>
@@ -16177,7 +16130,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="307" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:15">
       <c r="A307" t="s">
         <v>573</v>
       </c>
@@ -16224,7 +16177,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="308" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:15">
       <c r="A308" t="s">
         <v>573</v>
       </c>
@@ -16271,7 +16224,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="309" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:15">
       <c r="A309" t="s">
         <v>573</v>
       </c>
@@ -16318,7 +16271,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="310" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:15">
       <c r="A310" t="s">
         <v>573</v>
       </c>
@@ -16365,7 +16318,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="311" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:15">
       <c r="A311" t="s">
         <v>573</v>
       </c>
@@ -16412,7 +16365,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="312" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:15">
       <c r="A312" t="s">
         <v>573</v>
       </c>
@@ -16459,7 +16412,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="313" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:15">
       <c r="A313" t="s">
         <v>587</v>
       </c>
@@ -16500,7 +16453,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="314" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:15">
       <c r="A314" t="s">
         <v>587</v>
       </c>
@@ -16547,7 +16500,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="315" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:15">
       <c r="A315" t="s">
         <v>587</v>
       </c>
@@ -16594,7 +16547,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="316" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:15">
       <c r="A316" t="s">
         <v>587</v>
       </c>
@@ -16641,7 +16594,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="317" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:15">
       <c r="A317" t="s">
         <v>587</v>
       </c>
@@ -16688,7 +16641,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="318" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:15">
       <c r="A318" t="s">
         <v>595</v>
       </c>
@@ -16729,7 +16682,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="319" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:15">
       <c r="A319" t="s">
         <v>595</v>
       </c>
@@ -16776,7 +16729,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="320" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:15">
       <c r="A320" t="s">
         <v>599</v>
       </c>
@@ -16817,7 +16770,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="321" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:15">
       <c r="A321" t="s">
         <v>601</v>
       </c>
@@ -16858,7 +16811,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="322" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:15">
       <c r="A322" t="s">
         <v>601</v>
       </c>
@@ -16905,7 +16858,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="323" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:15">
       <c r="A323" t="s">
         <v>601</v>
       </c>
@@ -16952,7 +16905,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="324" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:15">
       <c r="A324" t="s">
         <v>601</v>
       </c>
@@ -16999,7 +16952,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="325" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:15">
       <c r="A325" t="s">
         <v>601</v>
       </c>
@@ -17046,7 +16999,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="326" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:15">
       <c r="A326" t="s">
         <v>601</v>
       </c>
@@ -17093,7 +17046,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="327" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:15">
       <c r="A327" t="s">
         <v>601</v>
       </c>
@@ -17140,7 +17093,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="328" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:15">
       <c r="A328" t="s">
         <v>601</v>
       </c>
@@ -17187,7 +17140,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="329" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:15">
       <c r="A329" t="s">
         <v>601</v>
       </c>
@@ -17234,7 +17187,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="330" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:15">
       <c r="A330" t="s">
         <v>601</v>
       </c>
@@ -17281,7 +17234,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="331" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:15">
       <c r="A331" t="s">
         <v>621</v>
       </c>
@@ -17322,7 +17275,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="332" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:15">
       <c r="A332" t="s">
         <v>621</v>
       </c>
@@ -17369,7 +17322,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="333" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:15">
       <c r="A333" t="s">
         <v>621</v>
       </c>
@@ -17416,7 +17369,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="334" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:15">
       <c r="A334" t="s">
         <v>621</v>
       </c>
@@ -17463,7 +17416,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="335" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:15">
       <c r="A335" t="s">
         <v>621</v>
       </c>
@@ -17510,7 +17463,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="336" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:15">
       <c r="A336" t="s">
         <v>621</v>
       </c>
@@ -17557,7 +17510,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="337" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:15">
       <c r="A337" t="s">
         <v>632</v>
       </c>
@@ -17598,7 +17551,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="338" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:15">
       <c r="A338" t="s">
         <v>632</v>
       </c>
@@ -17645,7 +17598,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="339" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:15">
       <c r="A339" t="s">
         <v>635</v>
       </c>
@@ -17686,7 +17639,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="340" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:15">
       <c r="A340" t="s">
         <v>635</v>
       </c>
@@ -17733,7 +17686,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="341" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:15">
       <c r="A341" t="s">
         <v>635</v>
       </c>
@@ -17780,7 +17733,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="342" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:15">
       <c r="A342" t="s">
         <v>641</v>
       </c>
@@ -17821,7 +17774,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="343" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:15">
       <c r="A343" t="s">
         <v>644</v>
       </c>
@@ -17862,7 +17815,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="344" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:15">
       <c r="A344" t="s">
         <v>647</v>
       </c>
@@ -17903,7 +17856,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="345" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:15">
       <c r="A345" t="s">
         <v>647</v>
       </c>
@@ -17950,7 +17903,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="346" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:15">
       <c r="A346" t="s">
         <v>647</v>
       </c>
@@ -17997,7 +17950,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="347" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:15">
       <c r="A347" t="s">
         <v>647</v>
       </c>
@@ -18044,7 +17997,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="348" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:15">
       <c r="A348" t="s">
         <v>652</v>
       </c>
@@ -18085,7 +18038,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="349" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:15">
       <c r="A349" t="s">
         <v>654</v>
       </c>
@@ -18126,7 +18079,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="350" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:15">
       <c r="A350" t="s">
         <v>657</v>
       </c>
@@ -18167,7 +18120,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="351" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:15">
       <c r="A351" t="s">
         <v>660</v>
       </c>
@@ -18208,7 +18161,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="352" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:15">
       <c r="A352" t="s">
         <v>660</v>
       </c>
@@ -18255,7 +18208,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="353" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:15">
       <c r="A353" t="s">
         <v>660</v>
       </c>
@@ -18302,7 +18255,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="354" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:15">
       <c r="A354" t="s">
         <v>660</v>
       </c>
@@ -18349,7 +18302,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="355" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:15">
       <c r="A355" t="s">
         <v>665</v>
       </c>
@@ -18390,7 +18343,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="356" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:15">
       <c r="A356" t="s">
         <v>665</v>
       </c>
@@ -18437,7 +18390,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="357" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:15">
       <c r="A357" t="s">
         <v>665</v>
       </c>
@@ -18484,7 +18437,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="358" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:15">
       <c r="A358" t="s">
         <v>669</v>
       </c>
@@ -18525,7 +18478,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="359" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:15">
       <c r="A359" t="s">
         <v>669</v>
       </c>
@@ -18572,7 +18525,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="360" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:15">
       <c r="A360" t="s">
         <v>672</v>
       </c>
@@ -18613,7 +18566,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="361" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:15">
       <c r="A361" t="s">
         <v>672</v>
       </c>
@@ -18660,7 +18613,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="362" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:15">
       <c r="A362" t="s">
         <v>676</v>
       </c>
@@ -18702,7 +18655,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P362" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:P362"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>